<commit_message>
Hiện thị tin tưc
</commit_message>
<xml_diff>
--- a/Book1 (version 1).xlsx
+++ b/Book1 (version 1).xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\du.nm165913\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D38BD8C1-DAA9-4C8D-909E-2754BB9AD39E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" activeTab="16" xr2:uid="{2F1BC66B-2AED-48DC-8889-27C5D7BFFAF2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -35,8 +29,7 @@
     <sheet name="delete user boi admin" sheetId="20" r:id="rId20"/>
     <sheet name="delete du an boi admin" sheetId="21" r:id="rId21"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -140,9 +133,6 @@
     <t>kieu</t>
   </si>
   <si>
-    <t>/api/sanpham/getnsanpham?id=</t>
-  </si>
-  <si>
     <t>id dc truyen vao param va lay 10sp co id nho hon id truyen vao</t>
   </si>
   <si>
@@ -334,11 +324,14 @@
   <si>
     <t>/api/duan/deletebyadmin</t>
   </si>
+  <si>
+    <t>/api/sanpham/getnsanpham?id=&amp;&amp;id_loaisp=</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -430,7 +423,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -482,7 +475,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -676,14 +669,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62747301-8F23-45A4-A2B5-935AD074F555}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -742,7 +735,7 @@
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -751,7 +744,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1080A52E-A782-4A1E-8B6D-9EECC04C9A53}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -762,7 +755,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -780,12 +773,12 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -809,7 +802,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080B344E-21E2-4586-B51C-BE9F92EBD3C0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -820,7 +813,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -838,12 +831,12 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -868,18 +861,18 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" t="s">
         <v>59</v>
-      </c>
-      <c r="G14" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" t="s">
         <v>61</v>
-      </c>
-      <c r="G15" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
@@ -893,7 +886,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B22734-4608-468C-AD78-D1087E9696E0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -904,7 +897,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -922,12 +915,12 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -947,7 +940,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -957,7 +950,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -966,7 +959,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAFBBB7-B367-432E-B3B9-933977EA7F2C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -977,7 +970,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -1002,7 +995,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -1026,7 +1019,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD4B2AB-7890-487D-9857-DE3E2CD72E1C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1037,7 +1030,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -1057,17 +1050,17 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1095,7 +1088,7 @@
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1104,7 +1097,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F0026D-7793-4DE8-BC3C-10141B692002}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1115,7 +1108,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -1135,7 +1128,7 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -1145,7 +1138,7 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -1164,7 +1157,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842263BA-28EF-4B12-8D52-35B12BC2FB4A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1175,7 +1168,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -1195,22 +1188,22 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -1220,7 +1213,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G11" t="s">
         <v>16</v>
@@ -1228,7 +1221,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G12" t="s">
         <v>16</v>
@@ -1236,7 +1229,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G13" t="s">
         <v>16</v>
@@ -1252,7 +1245,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G15" t="s">
         <v>16</v>
@@ -1260,7 +1253,7 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s">
         <v>16</v>
@@ -1268,7 +1261,7 @@
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s">
         <v>16</v>
@@ -1276,7 +1269,7 @@
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G18" t="s">
         <v>16</v>
@@ -1284,7 +1277,7 @@
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G19" t="s">
         <v>16</v>
@@ -1311,10 +1304,10 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA264BD-FF34-4ECD-B148-D6D9CB00CC07}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -1322,7 +1315,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -1342,17 +1335,17 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1360,12 +1353,12 @@
         <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -1389,7 +1382,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23D9FB5-9FED-4D7B-97D3-1D392B0773EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1400,7 +1393,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -1420,7 +1413,7 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -1430,7 +1423,7 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -1449,7 +1442,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E18AC640-FD97-4F16-BACC-BA23BD88E0D9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1460,7 +1453,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -1480,7 +1473,7 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -1491,7 +1484,7 @@
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -1515,7 +1508,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BACE40D-6969-4043-ACB4-9B038D8D3EDD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1604,7 +1597,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A4CE41-2AF9-4FB3-B8D3-EA1ECE048F60}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1615,7 +1608,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -1633,12 +1626,12 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -1646,7 +1639,7 @@
         <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -1670,7 +1663,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFF3C549-CF18-4D24-9FBA-D8A7A3461557}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -1681,7 +1674,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -1699,12 +1692,12 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -1712,7 +1705,7 @@
         <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -1736,18 +1729,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B615D2E-EA7B-4F88-A95B-C08CEB8B7C3C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -1768,12 +1761,12 @@
         <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -1794,7 +1787,7 @@
         <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -1828,7 +1821,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E387F1E-02FE-47F0-A861-BC29BD003508}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1860,7 +1853,7 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -1886,7 +1879,7 @@
         <v>27</v>
       </c>
       <c r="H11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1895,7 +1888,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79487E0-604D-44DE-B65F-10864A3B0CAB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1906,7 +1899,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -1927,12 +1920,12 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -1958,7 +1951,7 @@
         <v>20</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -1968,7 +1961,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -1978,7 +1971,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1987,7 +1980,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB7EEA81-E1C2-41E2-8004-48ED25F2942B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1998,7 +1991,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -2016,7 +2009,7 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -2031,7 +2024,7 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -2042,7 +2035,7 @@
         <v>27</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2051,7 +2044,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F8F9CEB-0E43-4C23-85CD-840AB9E3012F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2062,7 +2055,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -2080,7 +2073,7 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -2106,7 +2099,7 @@
         <v>20</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -2116,7 +2109,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -2130,7 +2123,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF41776-C044-4182-B3B7-C0AAC8D35EEE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G10"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -2141,7 +2134,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -2159,7 +2152,7 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -2182,7 +2175,7 @@
         <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2191,7 +2184,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E011DD5B-2E40-48BF-B8D6-1BB526D1DC51}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -2202,7 +2195,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -2222,7 +2215,7 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -2230,7 +2223,7 @@
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Sửa lỗi thiếu kiểm tra đăng nhập
</commit_message>
<xml_diff>
--- a/Book1 (version 1).xlsx
+++ b/Book1 (version 1).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" tabRatio="911" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -669,7 +669,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1732,7 +1732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1984,7 +1984,7 @@
   <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2048,7 +2048,7 @@
   <dimension ref="B2:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2126,8 +2126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>